<commit_message>
back up 13 oct 2021
</commit_message>
<xml_diff>
--- a/data/external/sra_ras_sum/sierra_data_summary_2020.xlsx
+++ b/data/external/sra_ras_sum/sierra_data_summary_2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2001_bulk_data" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="293">
   <si>
     <t>PM</t>
   </si>
@@ -912,6 +912,9 @@
   <si>
     <t>lyr_bot</t>
   </si>
+  <si>
+    <t>ID_sra</t>
+  </si>
 </sst>
 </file>
 
@@ -1412,7 +1415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1422,7 +1425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -5136,7 +5139,7 @@
   <dimension ref="A1:V125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5176,7 +5179,7 @@
         <v>287</v>
       </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -12090,7 +12093,7 @@
         <v>GRrf_11</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" ref="D98:D129" si="13">E98&amp;IF(G98="PP","pp",IF(G98="WF","wf",IF(G98="RF","rf")))&amp;"_"&amp;H98&amp;"_"&amp;N98&amp;"-"&amp;O98</f>
+        <f t="shared" ref="D98:D125" si="13">E98&amp;IF(G98="PP","pp",IF(G98="WF","wf",IF(G98="RF","rf")))&amp;"_"&amp;H98&amp;"_"&amp;N98&amp;"-"&amp;O98</f>
         <v>GRrf_1_0-13</v>
       </c>
       <c r="E98" t="str">
@@ -19653,8 +19656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA44"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -19727,7 +19730,7 @@
         <v>287</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="C1" t="s">
         <v>285</v>

</xml_diff>